<commit_message>
created the first time
</commit_message>
<xml_diff>
--- a/知识硬盘.xlsx
+++ b/知识硬盘.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>python</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,7 +86,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>namedtuple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>os</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -331,7 +339,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -512,6 +520,9 @@
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -530,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -815,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -852,8 +863,8 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="66" t="s">
-        <v>15</v>
+      <c r="A2" s="60" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -875,23 +886,27 @@
       <c r="Q2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="60" t="s">
+      <c r="R2" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
     </row>
     <row r="3" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="18"/>
+      <c r="A3" s="60" t="s">
+        <v>15</v>
+      </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="E3" s="67" t="s">
+        <v>17</v>
+      </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
@@ -983,20 +998,20 @@
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="62"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="21"/>
       <c r="I8" s="31"/>
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
-      <c r="L8" s="63" t="s">
+      <c r="L8" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="62"/>
+      <c r="M8" s="63"/>
       <c r="N8" s="33"/>
       <c r="O8" s="33"/>
       <c r="P8" s="34"/>
@@ -1005,8 +1020,8 @@
       <c r="A9" s="22"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="23"/>
@@ -1015,8 +1030,8 @@
       </c>
       <c r="J9" s="33"/>
       <c r="K9" s="33"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
       <c r="N9" s="32"/>
       <c r="O9" s="32"/>
       <c r="P9" s="36"/>
@@ -1281,20 +1296,20 @@
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="E24" s="62"/>
+      <c r="E24" s="63"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="8"/>
       <c r="I24" s="45"/>
       <c r="J24" s="46"/>
       <c r="K24" s="46"/>
-      <c r="L24" s="64" t="s">
+      <c r="L24" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="M24" s="65"/>
+      <c r="M24" s="66"/>
       <c r="N24" s="47"/>
       <c r="O24" s="47"/>
       <c r="P24" s="48"/>
@@ -1303,16 +1318,16 @@
       <c r="A25" s="9"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="10"/>
       <c r="I25" s="49"/>
       <c r="J25" s="47"/>
       <c r="K25" s="47"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="66"/>
       <c r="N25" s="50"/>
       <c r="O25" s="50"/>
       <c r="P25" s="51"/>

</xml_diff>